<commit_message>
PCB connector Bill revised
</commit_message>
<xml_diff>
--- a/PCB connector Bill.xlsx
+++ b/PCB connector Bill.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Item #</t>
   </si>
@@ -47,43 +47,25 @@
     <t>Manufactur Part#</t>
   </si>
   <si>
-    <t>538-51216-0200</t>
-  </si>
-  <si>
     <t>51216-0200</t>
   </si>
   <si>
     <t>Receptacle Housing</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>1.35 * 1.3</t>
-  </si>
-  <si>
-    <t>538-51217-0205</t>
-  </si>
-  <si>
     <t>Terminal Retainer</t>
   </si>
   <si>
     <t>51217-0205</t>
   </si>
   <si>
-    <t>2.32 * 1.3</t>
-  </si>
-  <si>
     <t>Vertical Header</t>
   </si>
   <si>
-    <t>538-55755-0219</t>
-  </si>
-  <si>
     <t>55755-0219</t>
   </si>
   <si>
-    <t>4.79 * 1.3</t>
+    <t>CAD</t>
   </si>
 </sst>
 </file>
@@ -100,13 +82,16 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
       <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,15 +111,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,12 +416,12 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
@@ -467,14 +454,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -483,21 +470,21 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>1.35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
+      <c r="A3" s="1">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -506,21 +493,21 @@
         <v>0.23200000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
+      <c r="A4" s="1">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -529,16 +516,22 @@
         <v>0.47899999999999998</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>4.79</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>